<commit_message>
Added the documentation for Excel service.
</commit_message>
<xml_diff>
--- a/docs/services/spreadsheets/needs2.xlsx
+++ b/docs/services/spreadsheets/needs2.xlsx
@@ -164,11 +164,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -683,501 +682,501 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="20.7109375"/>
-    <col customWidth="1" min="6" max="6" style="1" width="20.7109375"/>
-    <col customWidth="1" min="7" max="7" style="2" width="20.7109375"/>
-    <col customWidth="1" min="8" max="10" width="20.7109375"/>
+    <col customWidth="1" min="2" max="6" width="20.7109375"/>
+    <col customWidth="1" min="7" max="7" style="1" width="20.7109375"/>
+    <col customWidth="1" min="8" max="8" style="2" width="20.7109375"/>
+    <col customWidth="1" min="9" max="11" width="20.7109375"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1">
+      <c r="B1">
         <v>1001</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>44713</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>44743</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2">
+      <c r="B2">
         <v>1002</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>44714</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>44744</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3">
+      <c r="B3">
         <v>1003</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>44715</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>44745</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4">
+      <c r="B4">
         <v>1004</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>44716</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>44746</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5">
+      <c r="B5">
         <v>1005</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>44717</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>44747</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6">
+      <c r="B6">
         <v>1006</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>44718</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>44748</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7">
+      <c r="B7">
         <v>1007</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>44719</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>44749</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8">
+      <c r="B8">
         <v>1008</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>44720</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>44750</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9">
+      <c r="B9">
         <v>1009</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>44721</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>44751</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10">
+      <c r="B10">
         <v>1010</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>44722</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>44752</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11">
+      <c r="B11">
         <v>1011</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>44723</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>44753</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12">
+      <c r="B12">
         <v>1012</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>44724</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>44754</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13">
+      <c r="B13">
         <v>1013</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>44725</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>44755</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14">
+      <c r="B14">
         <v>1014</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>44726</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>44756</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15">
+      <c r="B15">
         <v>1015</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>44727</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>44757</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16">
+      <c r="B16">
         <v>1016</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>44728</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>44758</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17">
+      <c r="B17">
         <v>1017</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>44729</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>44759</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18">
+      <c r="B18">
         <v>1018</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>44730</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>44760</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19">
+      <c r="B19">
         <v>1019</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>44731</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>44761</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20">
+      <c r="B20">
         <v>1020</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="D20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>44732</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>44762</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>